<commit_message>
Database testing with JDBC.
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/Resources/CampusReport.xlsx
+++ b/src/test/java/ApachePOI/Resources/CampusReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
   <si>
     <t>9f73dee0-bec7-4871-af25-fceebc83d722</t>
   </si>
@@ -24,6 +24,30 @@
   </si>
   <si>
     <t>PT5.4588302S</t>
+  </si>
+  <si>
+    <t>b0749336-cacc-4ff8-9b32-265c9d23ada0</t>
+  </si>
+  <si>
+    <t>States Testing with JDBC</t>
+  </si>
+  <si>
+    <t>FAILED</t>
+  </si>
+  <si>
+    <t>PT7.7153474S</t>
+  </si>
+  <si>
+    <t>43a3213f-c717-4a4c-ab6d-16ad6178c445</t>
+  </si>
+  <si>
+    <t>PT6.6610874S</t>
+  </si>
+  <si>
+    <t>85b5aaf4-4198-4368-a167-52852f45d5ed</t>
+  </si>
+  <si>
+    <t>PT6.4608688S</t>
   </si>
 </sst>
 </file>
@@ -68,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -94,6 +118,126 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D2" t="n" s="0">
+        <v>45026.84047579861</v>
+      </c>
+      <c r="E2" t="n" s="0">
+        <v>45026.84056510417</v>
+      </c>
+      <c r="F2" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>45026.84047579861</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>45026.84056510417</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D4" t="n" s="0">
+        <v>45026.841017025465</v>
+      </c>
+      <c r="E4" t="n" s="0">
+        <v>45026.84109412037</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D5" t="n" s="0">
+        <v>45026.841017025465</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>45026.84109412037</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D6" t="n" s="0">
+        <v>45026.84403097222</v>
+      </c>
+      <c r="E6" t="n" s="0">
+        <v>45026.844105752316</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <v>45026.84403097222</v>
+      </c>
+      <c r="E7" t="n" s="0">
+        <v>45026.844105752316</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Arguments added for Chrome (for Jenkins).
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/Resources/CampusReport.xlsx
+++ b/src/test/java/ApachePOI/Resources/CampusReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>9f73dee0-bec7-4871-af25-fceebc83d722</t>
   </si>
@@ -48,6 +48,21 @@
   </si>
   <si>
     <t>PT6.4608688S</t>
+  </si>
+  <si>
+    <t>9c5c7be0-5623-4c31-96cb-89cba41271c5</t>
+  </si>
+  <si>
+    <t>PT4.9319502S</t>
+  </si>
+  <si>
+    <t>9478cb78-099a-404d-8883-61f48c1d5fdd</t>
+  </si>
+  <si>
+    <t>Create Country</t>
+  </si>
+  <si>
+    <t>PT7.1877896S</t>
   </si>
 </sst>
 </file>
@@ -92,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -238,6 +253,46 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n" s="0">
+        <v>45048.84917055556</v>
+      </c>
+      <c r="E8" t="n" s="0">
+        <v>45048.84922762732</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <v>45048.849267743055</v>
+      </c>
+      <c r="E9" t="n" s="0">
+        <v>45048.8493509375</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>